<commit_message>
Updated some more of the tables and figures
</commit_message>
<xml_diff>
--- a/Hjemsendelse 05-11-2025.xlsx
+++ b/Hjemsendelse 05-11-2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariussmidt/Desktop/BA/Bachelor/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hansandersen/Desktop/UNI/Bachelor/Bachelor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DCBF6E-CC18-3C4A-BA25-4405BEF85BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0EB320-A20A-D149-AFAC-CB7BA8EBD9D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="500" windowWidth="24700" windowHeight="15880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model results" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="22">
   <si>
     <t>sqm</t>
   </si>
@@ -107,7 +107,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="170" formatCode="_(* #,##0_);_(* \(#.##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +124,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -146,10 +157,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -157,8 +169,17 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -177,7 +198,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="da-DK"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -214,7 +235,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="da-DK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -614,7 +635,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="da-DK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="716659695"/>
@@ -677,7 +698,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="da-DK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="668002352"/>
@@ -719,13 +740,12 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="da-DK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -733,6 +753,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -756,7 +777,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="da-DK"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -770,7 +791,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="da-DK"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -807,7 +828,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="da-DK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1455,7 +1476,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="da-DK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="80862768"/>
@@ -1517,7 +1538,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="da-DK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="80920880"/>
@@ -1534,7 +1555,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1542,6 +1562,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1565,7 +1586,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="da-DK"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1579,7 +1600,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="da-DK"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1616,7 +1637,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="da-DK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2264,7 +2285,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="da-DK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="80862768"/>
@@ -2326,7 +2347,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="da-DK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="80920880"/>
@@ -2343,7 +2364,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2351,6 +2371,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2374,7 +2395,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="da-DK"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4057,16 +4078,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4093,16 +4114,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>196850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>196850</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4129,16 +4150,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5688,15 +5709,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G88"/>
+  <dimension ref="A1:N88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Z14" sqref="Z14"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="N50" sqref="N50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="6" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="14" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -6466,7 +6488,7 @@
         <v>69.433270444763195</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>51</v>
       </c>
@@ -6490,7 +6512,7 @@
         <v>67.678191565873732</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>52</v>
       </c>
@@ -6514,7 +6536,7 @@
         <v>67.132898618744804</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>53</v>
       </c>
@@ -6538,7 +6560,7 @@
         <v>68.661494877803776</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>54</v>
       </c>
@@ -6562,7 +6584,7 @@
         <v>67.402794232414806</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>55</v>
       </c>
@@ -6586,7 +6608,7 @@
         <v>66.938108260501821</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>56</v>
       </c>
@@ -6610,7 +6632,7 @@
         <v>67.263728257749293</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>57</v>
       </c>
@@ -6634,7 +6656,7 @@
         <v>66.739989914298945</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>58</v>
       </c>
@@ -6658,7 +6680,7 @@
         <v>66.520695629136384</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>59</v>
       </c>
@@ -6682,7 +6704,7 @@
         <v>66.032963144693056</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>60</v>
       </c>
@@ -6706,7 +6728,7 @@
         <v>65.584001377631836</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>61</v>
       </c>
@@ -6730,7 +6752,7 @@
         <v>65.065573040726719</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>62</v>
       </c>
@@ -6754,7 +6776,7 @@
         <v>63.624385375615802</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>63</v>
       </c>
@@ -6778,7 +6800,7 @@
         <v>63.287071316006504</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>64</v>
       </c>
@@ -6802,7 +6824,7 @@
         <v>63.844092593533283</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>65</v>
       </c>
@@ -6825,8 +6847,9 @@
         <f t="shared" si="0"/>
         <v>63.508441905938149</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I47" s="3"/>
+    </row>
+    <row r="48" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>66</v>
       </c>
@@ -6849,8 +6872,16 @@
         <f t="shared" si="0"/>
         <v>64.143990784488636</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I48" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5"/>
+    </row>
+    <row r="49" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>67</v>
       </c>
@@ -6873,8 +6904,26 @@
         <f t="shared" si="0"/>
         <v>64.091406663491199</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I49" s="4">
+        <v>3</v>
+      </c>
+      <c r="J49" s="4">
+        <v>4</v>
+      </c>
+      <c r="K49" s="4">
+        <v>5</v>
+      </c>
+      <c r="L49" s="4">
+        <v>7</v>
+      </c>
+      <c r="M49" s="4">
+        <v>10</v>
+      </c>
+      <c r="N49" s="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>68</v>
       </c>
@@ -6897,8 +6946,32 @@
         <f t="shared" si="0"/>
         <v>63.531698370162061</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I50" s="6">
+        <f>SUM(B44:B50)</f>
+        <v>104007</v>
+      </c>
+      <c r="J50" s="6">
+        <f>SUM(B43:B51)</f>
+        <v>132995</v>
+      </c>
+      <c r="K50" s="6">
+        <f>SUM(B42:B52)</f>
+        <v>167944</v>
+      </c>
+      <c r="L50" s="6">
+        <f>SUM(B40:B54)</f>
+        <v>221174</v>
+      </c>
+      <c r="M50" s="6">
+        <f>SUM(B37:B57)</f>
+        <v>295767</v>
+      </c>
+      <c r="N50" s="6">
+        <f>SUM(B33:B61)</f>
+        <v>385613</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>69</v>
       </c>
@@ -6922,7 +6995,7 @@
         <v>64.242319775724496</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>70</v>
       </c>
@@ -6946,7 +7019,7 @@
         <v>61.672693216939429</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>71</v>
       </c>
@@ -6970,7 +7043,7 @@
         <v>63.302354445187468</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>72</v>
       </c>
@@ -6994,7 +7067,7 @@
         <v>61.92735583857862</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>73</v>
       </c>
@@ -7018,7 +7091,7 @@
         <v>61.845930783583704</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>74</v>
       </c>
@@ -7042,7 +7115,7 @@
         <v>61.707510155383652</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>75</v>
       </c>
@@ -7066,7 +7139,7 @@
         <v>60.181645382897067</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>76</v>
       </c>
@@ -7090,7 +7163,7 @@
         <v>60.794884920149478</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>77</v>
       </c>
@@ -7114,7 +7187,7 @@
         <v>60.118490359769353</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>78</v>
       </c>
@@ -7138,7 +7211,7 @@
         <v>60.245485176078851</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>79</v>
       </c>
@@ -7162,7 +7235,7 @@
         <v>59.632896475910378</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>80</v>
       </c>
@@ -7186,7 +7259,7 @@
         <v>60.413191481255623</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>81</v>
       </c>
@@ -7210,7 +7283,7 @@
         <v>60.271325242379874</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>82</v>
       </c>
@@ -7811,6 +7884,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I48:N48"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>